<commit_message>
[task] Fix method used for gathering timing of processes 	- Now gets timings for all processes in scheduler 	- Prints timing to text file on teardown
</commit_message>
<xml_diff>
--- a/Documentation/Frequency.xlsx
+++ b/Documentation/Frequency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brams\eclipse-workspace\ElevatorControlSystem\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D4D6F6-A5B6-49F7-9C5B-E4FB5EAB3ECB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5783718B-5747-4751-ACFE-39064BD62D3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="13" xr2:uid="{388977CB-29F1-40BC-8A21-2391053F826C}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>CONFIG_MODE</t>
   </si>
@@ -449,7 +449,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +527,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +604,7 @@
         <v>21802032700</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B22" si="0">A4 - A3</f>
+        <f t="shared" ref="B3:B20" si="0">A4 - A3</f>
         <v>5999677400</v>
       </c>
     </row>
@@ -776,7 +776,7 @@
   <dimension ref="A1:C134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2004,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2045,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,6 +2069,9 @@
       <c r="B2" t="s">
         <v>15</v>
       </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2080,7 +2083,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,6 +2110,9 @@
       <c r="B2" t="s">
         <v>15</v>
       </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2118,7 +2124,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2142,6 +2148,9 @@
       <c r="B2" t="s">
         <v>15</v>
       </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2153,7 +2162,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,7 +2250,7 @@
         <v>27804847700</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B42" si="0">A4 - A3</f>
+        <f t="shared" ref="B3:B41" si="0">A4 - A3</f>
         <v>11998415600</v>
       </c>
     </row>
@@ -2602,7 +2611,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2643,7 +2652,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2681,7 +2690,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>